<commit_message>
Moving XML library files around. Completed S3 error audit.
</commit_message>
<xml_diff>
--- a/source/_docs/Error Codes - AWS Toolkit - S3.xlsx
+++ b/source/_docs/Error Codes - AWS Toolkit - S3.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
     <t>Code</t>
   </si>
@@ -153,6 +153,27 @@
   </si>
   <si>
     <t>NoSuchBucketPolicy - The bucket does not have a policy.</t>
+  </si>
+  <si>
+    <t>InvalidBucketState - The request is not valid with the current state of the bucket.</t>
+  </si>
+  <si>
+    <t>InvalidEncryptionAlgorithmError - The encryption request you specified is not valid. The valid value is AES256.</t>
+  </si>
+  <si>
+    <t>InvalidObjectState - The operation is not valid for the current state of the object.</t>
+  </si>
+  <si>
+    <t>InvalidRequest - Some part of the specified request is invalid.</t>
+  </si>
+  <si>
+    <t>NoSuchLifecycleConfiguration - The lifecycle configuration does not exist.</t>
+  </si>
+  <si>
+    <t>RestoreAlreadyInProgress - Object restore is already in progress.</t>
+  </si>
+  <si>
+    <t>ServiceUnavailable - Reduce your request rate.</t>
   </si>
 </sst>
 </file>
@@ -528,10 +549,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B42"/>
+  <dimension ref="A1:B49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -876,6 +897,62 @@
         <v>42</v>
       </c>
     </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="3">
+        <v>412341</v>
+      </c>
+      <c r="B43" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="3">
+        <v>412342</v>
+      </c>
+      <c r="B44" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="3">
+        <v>412343</v>
+      </c>
+      <c r="B45" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="3">
+        <v>412344</v>
+      </c>
+      <c r="B46" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="3">
+        <v>412345</v>
+      </c>
+      <c r="B47" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="3">
+        <v>412346</v>
+      </c>
+      <c r="B48" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="3">
+        <v>412347</v>
+      </c>
+      <c r="B49" t="s">
+        <v>49</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Implemented more 'Get Bucket' VIs
</commit_message>
<xml_diff>
--- a/source/_docs/Error Codes - AWS Toolkit - S3.xlsx
+++ b/source/_docs/Error Codes - AWS Toolkit - S3.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t>Code</t>
   </si>
@@ -174,6 +174,9 @@
   </si>
   <si>
     <t>ServiceUnavailable - Reduce your request rate.</t>
+  </si>
+  <si>
+    <t>NoSuchWebsiteConfiguration - The specified bucket does not have a website configuration.</t>
   </si>
 </sst>
 </file>
@@ -549,10 +552,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B49"/>
+  <dimension ref="A1:B50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="B52" sqref="B52"/>
+      <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -953,6 +956,14 @@
         <v>49</v>
       </c>
     </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="3">
+        <v>412348</v>
+      </c>
+      <c r="B50" t="s">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>